<commit_message>
Task Scheduler updates prediction every day
</commit_message>
<xml_diff>
--- a/prediction_record.xlsx
+++ b/prediction_record.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4680" yWindow="4680" windowWidth="28785" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-26670" yWindow="3240" windowWidth="25635" windowHeight="14445" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -458,10 +458,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62:E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -2394,8 +2394,13 @@
           <t>Calgary Hitmen</t>
         </is>
       </c>
-      <c r="F58" t="n">
-        <v/>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Calgary Hitmen</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -2422,8 +2427,13 @@
           <t>Edmonton Oil Kings</t>
         </is>
       </c>
-      <c r="F59" t="n">
-        <v/>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Lethbridge Hurricanes</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -2450,8 +2460,13 @@
           <t>Tri-City Americans</t>
         </is>
       </c>
-      <c r="F60" t="n">
-        <v/>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Wenatchee Wild</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -2478,7 +2493,124 @@
           <t>Spokane Chiefs</t>
         </is>
       </c>
-      <c r="F61" t="n">
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Spokane Chiefs</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>1021608</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Tue, Jan 7, 2025</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Lethbridge Hurricanes</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Moose Jaw Warriors</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Moose Jaw Warriors</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>1021610</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Tue, Jan 7, 2025</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Red Deer Rebels</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Saskatoon Blades</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Saskatoon Blades</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>1021609</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Tue, Jan 7, 2025</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Prince George Cougars</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Vancouver Giants</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Vancouver Giants</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>1021611</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Tue, Jan 7, 2025</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Seattle Thunderbirds</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Victoria Royals</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Victoria Royals</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Now uses KFold Validation
</commit_message>
<xml_diff>
--- a/prediction_record.xlsx
+++ b/prediction_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0bd5acfa1e98a521/Documents/A-Z Machine Learning-Calebs-/A-Z_Machine-Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_03498AB6D612B7E5862D0BBBEA32115B5D093391" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_0E123C47D5482C6F6D72103554322E3B1D001FF7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="50">
   <si>
     <t>GameID</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>Fri, Jan 17, 2025</t>
+  </si>
+  <si>
+    <t>Sat, Jan 18, 2025</t>
   </si>
 </sst>
 </file>
@@ -565,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:I118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="F112" sqref="F112"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="G118" sqref="G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +636,7 @@
       </c>
       <c r="I2" s="2" t="str">
         <f>TEXT((SUM(G:G)/(COUNTA(G:G)-1)), "0.00%")</f>
-        <v>60.82%</v>
+        <v>60.19%</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2860,6 +2863,12 @@
       <c r="E99" t="s">
         <v>19</v>
       </c>
+      <c r="F99" t="s">
+        <v>19</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
@@ -2877,6 +2886,12 @@
       <c r="E100" t="s">
         <v>12</v>
       </c>
+      <c r="F100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101">
@@ -2894,6 +2909,12 @@
       <c r="E101" t="s">
         <v>16</v>
       </c>
+      <c r="F101" t="s">
+        <v>16</v>
+      </c>
+      <c r="G101">
+        <v>1</v>
+      </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102">
@@ -2911,6 +2932,12 @@
       <c r="E102" t="s">
         <v>13</v>
       </c>
+      <c r="F102" t="s">
+        <v>13</v>
+      </c>
+      <c r="G102">
+        <v>1</v>
+      </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103">
@@ -2928,6 +2955,12 @@
       <c r="E103" t="s">
         <v>32</v>
       </c>
+      <c r="F103" t="s">
+        <v>26</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104">
@@ -2945,6 +2978,12 @@
       <c r="E104" t="s">
         <v>18</v>
       </c>
+      <c r="F104" t="s">
+        <v>18</v>
+      </c>
+      <c r="G104">
+        <v>1</v>
+      </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105">
@@ -2962,6 +3001,12 @@
       <c r="E105" t="s">
         <v>27</v>
       </c>
+      <c r="F105" t="s">
+        <v>27</v>
+      </c>
+      <c r="G105">
+        <v>1</v>
+      </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106">
@@ -2979,6 +3024,12 @@
       <c r="E106" t="s">
         <v>9</v>
       </c>
+      <c r="F106" t="s">
+        <v>22</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107">
@@ -2996,6 +3047,12 @@
       <c r="E107" t="s">
         <v>28</v>
       </c>
+      <c r="F107" t="s">
+        <v>21</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108">
@@ -3013,6 +3070,12 @@
       <c r="E108" t="s">
         <v>23</v>
       </c>
+      <c r="F108" t="s">
+        <v>23</v>
+      </c>
+      <c r="G108">
+        <v>1</v>
+      </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109">
@@ -3029,6 +3092,165 @@
       </c>
       <c r="E109" t="s">
         <v>17</v>
+      </c>
+      <c r="F109" t="s">
+        <v>29</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>1021658</v>
+      </c>
+      <c r="B110" t="s">
+        <v>49</v>
+      </c>
+      <c r="C110" t="s">
+        <v>14</v>
+      </c>
+      <c r="D110" t="s">
+        <v>16</v>
+      </c>
+      <c r="E110" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>1021659</v>
+      </c>
+      <c r="B111" t="s">
+        <v>49</v>
+      </c>
+      <c r="C111" t="s">
+        <v>11</v>
+      </c>
+      <c r="D111" t="s">
+        <v>15</v>
+      </c>
+      <c r="E111" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>1021662</v>
+      </c>
+      <c r="B112" t="s">
+        <v>49</v>
+      </c>
+      <c r="C112" t="s">
+        <v>12</v>
+      </c>
+      <c r="D112" t="s">
+        <v>19</v>
+      </c>
+      <c r="E112" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>1021657</v>
+      </c>
+      <c r="B113" t="s">
+        <v>49</v>
+      </c>
+      <c r="C113" t="s">
+        <v>26</v>
+      </c>
+      <c r="D113" t="s">
+        <v>32</v>
+      </c>
+      <c r="E113" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>1021656</v>
+      </c>
+      <c r="B114" t="s">
+        <v>49</v>
+      </c>
+      <c r="C114" t="s">
+        <v>22</v>
+      </c>
+      <c r="D114" t="s">
+        <v>35</v>
+      </c>
+      <c r="E114" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>1021660</v>
+      </c>
+      <c r="B115" t="s">
+        <v>49</v>
+      </c>
+      <c r="C115" t="s">
+        <v>21</v>
+      </c>
+      <c r="D115" t="s">
+        <v>28</v>
+      </c>
+      <c r="E115" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>1021661</v>
+      </c>
+      <c r="B116" t="s">
+        <v>49</v>
+      </c>
+      <c r="C116" t="s">
+        <v>23</v>
+      </c>
+      <c r="D116" t="s">
+        <v>27</v>
+      </c>
+      <c r="E116" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>1021663</v>
+      </c>
+      <c r="B117" t="s">
+        <v>49</v>
+      </c>
+      <c r="C117" t="s">
+        <v>20</v>
+      </c>
+      <c r="D117" t="s">
+        <v>24</v>
+      </c>
+      <c r="E117" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>1021664</v>
+      </c>
+      <c r="B118" t="s">
+        <v>49</v>
+      </c>
+      <c r="C118" t="s">
+        <v>29</v>
+      </c>
+      <c r="D118" t="s">
+        <v>17</v>
+      </c>
+      <c r="E118" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update predictions and stats
</commit_message>
<xml_diff>
--- a/prediction_record.xlsx
+++ b/prediction_record.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0bd5acfa1e98a521/Documents/A-Z Machine Learning-Calebs-/A-Z_Machine-Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_7F4D45A5573B25E4862D0B6BBAB52A555D0803D9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB43736B-8D7B-4D6C-A189-330C7F4E7A98}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_0E6DC1EB141243E4862D0B18E23523DF5C086F68" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D56AD6F-CA52-471D-A184-A2DE8A7DD649}"/>
   <bookViews>
     <workbookView xWindow="1395" yWindow="3465" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="62">
   <si>
     <t>GameID</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>Sat, Feb 1, 2025</t>
+  </si>
+  <si>
+    <t>Sun, Feb 2, 2025</t>
+  </si>
+  <si>
+    <t>Tue, Feb 4, 2025</t>
   </si>
 </sst>
 </file>
@@ -279,10 +285,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -602,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I180"/>
+  <dimension ref="A1:I187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="F171" sqref="F171"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="F185" sqref="F185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,7 +672,7 @@
       </c>
       <c r="I2" s="2" t="str">
         <f>TEXT((SUM(G:G)/(COUNTA(G:G)-1)), "0.00%")</f>
-        <v>63.91%</v>
+        <v>63.93%</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4553,6 +4555,12 @@
       <c r="E171" t="s">
         <v>9</v>
       </c>
+      <c r="F171" t="s">
+        <v>9</v>
+      </c>
+      <c r="G171">
+        <v>1</v>
+      </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172">
@@ -4570,6 +4578,12 @@
       <c r="E172" t="s">
         <v>27</v>
       </c>
+      <c r="F172" t="s">
+        <v>16</v>
+      </c>
+      <c r="G172">
+        <v>0</v>
+      </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173">
@@ -4587,6 +4601,12 @@
       <c r="E173" t="s">
         <v>15</v>
       </c>
+      <c r="F173" t="s">
+        <v>15</v>
+      </c>
+      <c r="G173">
+        <v>1</v>
+      </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174">
@@ -4604,6 +4624,12 @@
       <c r="E174" t="s">
         <v>24</v>
       </c>
+      <c r="F174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G174">
+        <v>0</v>
+      </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175">
@@ -4621,6 +4647,12 @@
       <c r="E175" t="s">
         <v>29</v>
       </c>
+      <c r="F175" t="s">
+        <v>29</v>
+      </c>
+      <c r="G175">
+        <v>1</v>
+      </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176">
@@ -4638,8 +4670,14 @@
       <c r="E176" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F176" t="s">
+        <v>35</v>
+      </c>
+      <c r="G176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>1021717</v>
       </c>
@@ -4655,8 +4693,14 @@
       <c r="E177" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F177" t="s">
+        <v>23</v>
+      </c>
+      <c r="G177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>1021718</v>
       </c>
@@ -4672,8 +4716,14 @@
       <c r="E178" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F178" t="s">
+        <v>12</v>
+      </c>
+      <c r="G178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>1021725</v>
       </c>
@@ -4689,8 +4739,14 @@
       <c r="E179" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F179" t="s">
+        <v>21</v>
+      </c>
+      <c r="G179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>1021726</v>
       </c>
@@ -4705,6 +4761,155 @@
       </c>
       <c r="E180" t="s">
         <v>17</v>
+      </c>
+      <c r="F180" t="s">
+        <v>18</v>
+      </c>
+      <c r="G180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>1021727</v>
+      </c>
+      <c r="B181" t="s">
+        <v>60</v>
+      </c>
+      <c r="C181" t="s">
+        <v>32</v>
+      </c>
+      <c r="D181" t="s">
+        <v>27</v>
+      </c>
+      <c r="E181" t="s">
+        <v>32</v>
+      </c>
+      <c r="F181" t="s">
+        <v>32</v>
+      </c>
+      <c r="G181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>1021729</v>
+      </c>
+      <c r="B182" t="s">
+        <v>60</v>
+      </c>
+      <c r="C182" t="s">
+        <v>13</v>
+      </c>
+      <c r="D182" t="s">
+        <v>14</v>
+      </c>
+      <c r="E182" t="s">
+        <v>13</v>
+      </c>
+      <c r="F182" t="s">
+        <v>13</v>
+      </c>
+      <c r="G182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>1021730</v>
+      </c>
+      <c r="B183" t="s">
+        <v>60</v>
+      </c>
+      <c r="C183" t="s">
+        <v>18</v>
+      </c>
+      <c r="D183" t="s">
+        <v>23</v>
+      </c>
+      <c r="E183" t="s">
+        <v>23</v>
+      </c>
+      <c r="F183" t="s">
+        <v>23</v>
+      </c>
+      <c r="G183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>1021728</v>
+      </c>
+      <c r="B184" t="s">
+        <v>60</v>
+      </c>
+      <c r="C184" t="s">
+        <v>22</v>
+      </c>
+      <c r="D184" t="s">
+        <v>17</v>
+      </c>
+      <c r="E184" t="s">
+        <v>22</v>
+      </c>
+      <c r="F184" t="s">
+        <v>22</v>
+      </c>
+      <c r="G184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>1021731</v>
+      </c>
+      <c r="B185" t="s">
+        <v>61</v>
+      </c>
+      <c r="C185" t="s">
+        <v>14</v>
+      </c>
+      <c r="D185" t="s">
+        <v>24</v>
+      </c>
+      <c r="E185" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>1021732</v>
+      </c>
+      <c r="B186" t="s">
+        <v>61</v>
+      </c>
+      <c r="C186" t="s">
+        <v>20</v>
+      </c>
+      <c r="D186" t="s">
+        <v>35</v>
+      </c>
+      <c r="E186" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>1021733</v>
+      </c>
+      <c r="B187" t="s">
+        <v>61</v>
+      </c>
+      <c r="C187" t="s">
+        <v>29</v>
+      </c>
+      <c r="D187" t="s">
+        <v>28</v>
+      </c>
+      <c r="E187" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify how models are picked
This is because it was a rough night for WHL predictions... reversed an if-statement
</commit_message>
<xml_diff>
--- a/prediction_record.xlsx
+++ b/prediction_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0bd5acfa1e98a521/Documents/A-Z Machine Learning-Calebs-/A-Z_Machine-Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_6CE98D9FD32235E4862D0BB45A350C235D082C75" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_64292D88D32235E4862D0B348AF30DF95C08ECB6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{934B84D2-8CFE-4409-A848-783F09B1631F}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30885" yWindow="2655" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="69">
   <si>
     <t>GameID</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>Fri, Feb 14, 2025</t>
+  </si>
+  <si>
+    <t>Sat, Feb 15, 2025</t>
   </si>
 </sst>
 </file>
@@ -303,6 +306,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -622,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I231"/>
+  <dimension ref="A1:I241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="H229" sqref="H229"/>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="I232" sqref="I232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +697,7 @@
       </c>
       <c r="I2" s="2" t="str">
         <f>TEXT((SUM(G:G)/(COUNTA(G:G)-1)), "0.00%")</f>
-        <v>64.09%</v>
+        <v>63.48%</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5746,6 +5753,12 @@
       <c r="E222" t="s">
         <v>9</v>
       </c>
+      <c r="F222" t="s">
+        <v>9</v>
+      </c>
+      <c r="G222">
+        <v>1</v>
+      </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223">
@@ -5763,6 +5776,12 @@
       <c r="E223" t="s">
         <v>12</v>
       </c>
+      <c r="F223" t="s">
+        <v>11</v>
+      </c>
+      <c r="G223">
+        <v>0</v>
+      </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224">
@@ -5780,8 +5799,14 @@
       <c r="E224" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F224" t="s">
+        <v>13</v>
+      </c>
+      <c r="G224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>1021769</v>
       </c>
@@ -5797,8 +5822,14 @@
       <c r="E225" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F225" t="s">
+        <v>27</v>
+      </c>
+      <c r="G225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>1021773</v>
       </c>
@@ -5814,8 +5845,14 @@
       <c r="E226" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F226" t="s">
+        <v>15</v>
+      </c>
+      <c r="G226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>1021768</v>
       </c>
@@ -5831,8 +5868,14 @@
       <c r="E227" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F227" t="s">
+        <v>17</v>
+      </c>
+      <c r="G227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>1021772</v>
       </c>
@@ -5848,8 +5891,14 @@
       <c r="E228" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F228" t="s">
+        <v>22</v>
+      </c>
+      <c r="G228">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>1021777</v>
       </c>
@@ -5865,8 +5914,14 @@
       <c r="E229" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F229" t="s">
+        <v>19</v>
+      </c>
+      <c r="G229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>1021775</v>
       </c>
@@ -5882,8 +5937,14 @@
       <c r="E230" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F230" t="s">
+        <v>20</v>
+      </c>
+      <c r="G230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>1021776</v>
       </c>
@@ -5897,6 +5958,182 @@
         <v>18</v>
       </c>
       <c r="E231" t="s">
+        <v>29</v>
+      </c>
+      <c r="F231" t="s">
+        <v>29</v>
+      </c>
+      <c r="G231">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>1021778</v>
+      </c>
+      <c r="B232" t="s">
+        <v>68</v>
+      </c>
+      <c r="C232" t="s">
+        <v>9</v>
+      </c>
+      <c r="D232" t="s">
+        <v>14</v>
+      </c>
+      <c r="E232" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>1021782</v>
+      </c>
+      <c r="B233" t="s">
+        <v>68</v>
+      </c>
+      <c r="C233" t="s">
+        <v>11</v>
+      </c>
+      <c r="D233" t="s">
+        <v>32</v>
+      </c>
+      <c r="E233" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>1021786</v>
+      </c>
+      <c r="B234" t="s">
+        <v>68</v>
+      </c>
+      <c r="C234" t="s">
+        <v>12</v>
+      </c>
+      <c r="D234" t="s">
+        <v>13</v>
+      </c>
+      <c r="E234" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>1021779</v>
+      </c>
+      <c r="B235" t="s">
+        <v>68</v>
+      </c>
+      <c r="C235" t="s">
+        <v>16</v>
+      </c>
+      <c r="D235" t="s">
+        <v>27</v>
+      </c>
+      <c r="E235" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>1021781</v>
+      </c>
+      <c r="B236" t="s">
+        <v>68</v>
+      </c>
+      <c r="C236" t="s">
+        <v>26</v>
+      </c>
+      <c r="D236" t="s">
+        <v>10</v>
+      </c>
+      <c r="E236" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>1021783</v>
+      </c>
+      <c r="B237" t="s">
+        <v>68</v>
+      </c>
+      <c r="C237" t="s">
+        <v>35</v>
+      </c>
+      <c r="D237" t="s">
+        <v>22</v>
+      </c>
+      <c r="E237" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>1021780</v>
+      </c>
+      <c r="B238" t="s">
+        <v>68</v>
+      </c>
+      <c r="C238" t="s">
+        <v>28</v>
+      </c>
+      <c r="D238" t="s">
+        <v>17</v>
+      </c>
+      <c r="E238" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>1021784</v>
+      </c>
+      <c r="B239" t="s">
+        <v>68</v>
+      </c>
+      <c r="C239" t="s">
+        <v>21</v>
+      </c>
+      <c r="D239" t="s">
+        <v>19</v>
+      </c>
+      <c r="E239" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>1021785</v>
+      </c>
+      <c r="B240" t="s">
+        <v>68</v>
+      </c>
+      <c r="C240" t="s">
+        <v>23</v>
+      </c>
+      <c r="D240" t="s">
+        <v>20</v>
+      </c>
+      <c r="E240" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>1021787</v>
+      </c>
+      <c r="B241" t="s">
+        <v>68</v>
+      </c>
+      <c r="C241" t="s">
+        <v>18</v>
+      </c>
+      <c r="D241" t="s">
+        <v>29</v>
+      </c>
+      <c r="E241" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update predictions, and revert changes
I was wrong, and ended up reversing my predictions. I just had a bad day a few day ago...
</commit_message>
<xml_diff>
--- a/prediction_record.xlsx
+++ b/prediction_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0bd5acfa1e98a521/Documents/A-Z Machine Learning-Calebs-/A-Z_Machine-Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="11_64292D88D32235E4862D0B348AF30DF95C08ECB6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{934B84D2-8CFE-4409-A848-783F09B1631F}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_174C5AA8D067C46F6D72103554322E3B7D88B6A9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3046F59-A911-4395-9E75-E8058ED28DA6}"/>
   <bookViews>
-    <workbookView xWindow="-30885" yWindow="2655" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="2700" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="72">
   <si>
     <t>GameID</t>
   </si>
@@ -240,6 +240,15 @@
   </si>
   <si>
     <t>Sat, Feb 15, 2025</t>
+  </si>
+  <si>
+    <t>Sun, Feb 16, 2025</t>
+  </si>
+  <si>
+    <t>Mon, Feb 17, 2025</t>
+  </si>
+  <si>
+    <t>Tue, Feb 18, 2025</t>
   </si>
 </sst>
 </file>
@@ -306,10 +315,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -629,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I241"/>
+  <dimension ref="A1:I253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
-      <selection activeCell="I232" sqref="I232"/>
+    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="I256" sqref="I256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,6 +650,8 @@
     <col min="6" max="6" width="23" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -697,7 +704,7 @@
       </c>
       <c r="I2" s="2" t="str">
         <f>TEXT((SUM(G:G)/(COUNTA(G:G)-1)), "0.00%")</f>
-        <v>63.48%</v>
+        <v>62.95%</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5983,6 +5990,12 @@
       <c r="E232" t="s">
         <v>9</v>
       </c>
+      <c r="F232" t="s">
+        <v>9</v>
+      </c>
+      <c r="G232">
+        <v>1</v>
+      </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233">
@@ -6000,6 +6013,12 @@
       <c r="E233" t="s">
         <v>32</v>
       </c>
+      <c r="F233" t="s">
+        <v>11</v>
+      </c>
+      <c r="G233">
+        <v>0</v>
+      </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234">
@@ -6017,6 +6036,12 @@
       <c r="E234" t="s">
         <v>13</v>
       </c>
+      <c r="F234" t="s">
+        <v>12</v>
+      </c>
+      <c r="G234">
+        <v>0</v>
+      </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235">
@@ -6034,6 +6059,12 @@
       <c r="E235" t="s">
         <v>27</v>
       </c>
+      <c r="F235" t="s">
+        <v>16</v>
+      </c>
+      <c r="G235">
+        <v>0</v>
+      </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236">
@@ -6051,6 +6082,12 @@
       <c r="E236" t="s">
         <v>26</v>
       </c>
+      <c r="F236" t="s">
+        <v>26</v>
+      </c>
+      <c r="G236">
+        <v>1</v>
+      </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237">
@@ -6068,6 +6105,12 @@
       <c r="E237" t="s">
         <v>22</v>
       </c>
+      <c r="F237" t="s">
+        <v>35</v>
+      </c>
+      <c r="G237">
+        <v>0</v>
+      </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238">
@@ -6085,6 +6128,12 @@
       <c r="E238" t="s">
         <v>28</v>
       </c>
+      <c r="F238" t="s">
+        <v>17</v>
+      </c>
+      <c r="G238">
+        <v>0</v>
+      </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239">
@@ -6102,6 +6151,12 @@
       <c r="E239" t="s">
         <v>21</v>
       </c>
+      <c r="F239" t="s">
+        <v>21</v>
+      </c>
+      <c r="G239">
+        <v>1</v>
+      </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240">
@@ -6119,8 +6174,14 @@
       <c r="E240" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F240" t="s">
+        <v>23</v>
+      </c>
+      <c r="G240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>1021787</v>
       </c>
@@ -6135,6 +6196,282 @@
       </c>
       <c r="E241" t="s">
         <v>29</v>
+      </c>
+      <c r="F241" t="s">
+        <v>18</v>
+      </c>
+      <c r="G241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>1021788</v>
+      </c>
+      <c r="B242" t="s">
+        <v>69</v>
+      </c>
+      <c r="C242" t="s">
+        <v>24</v>
+      </c>
+      <c r="D242" t="s">
+        <v>21</v>
+      </c>
+      <c r="E242" t="s">
+        <v>21</v>
+      </c>
+      <c r="F242" t="s">
+        <v>21</v>
+      </c>
+      <c r="G242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>1021792</v>
+      </c>
+      <c r="B243" t="s">
+        <v>70</v>
+      </c>
+      <c r="C243" t="s">
+        <v>14</v>
+      </c>
+      <c r="D243" t="s">
+        <v>11</v>
+      </c>
+      <c r="E243" t="s">
+        <v>11</v>
+      </c>
+      <c r="F243" t="s">
+        <v>11</v>
+      </c>
+      <c r="G243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>1021791</v>
+      </c>
+      <c r="B244" t="s">
+        <v>70</v>
+      </c>
+      <c r="C244" t="s">
+        <v>26</v>
+      </c>
+      <c r="D244" t="s">
+        <v>27</v>
+      </c>
+      <c r="E244" t="s">
+        <v>26</v>
+      </c>
+      <c r="F244" t="s">
+        <v>26</v>
+      </c>
+      <c r="G244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>1021794</v>
+      </c>
+      <c r="B245" t="s">
+        <v>70</v>
+      </c>
+      <c r="C245" t="s">
+        <v>15</v>
+      </c>
+      <c r="D245" t="s">
+        <v>16</v>
+      </c>
+      <c r="E245" t="s">
+        <v>16</v>
+      </c>
+      <c r="F245" t="s">
+        <v>16</v>
+      </c>
+      <c r="G245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>1021789</v>
+      </c>
+      <c r="B246" t="s">
+        <v>70</v>
+      </c>
+      <c r="C246" t="s">
+        <v>17</v>
+      </c>
+      <c r="D246" t="s">
+        <v>23</v>
+      </c>
+      <c r="E246" t="s">
+        <v>23</v>
+      </c>
+      <c r="F246" t="s">
+        <v>23</v>
+      </c>
+      <c r="G246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>1021795</v>
+      </c>
+      <c r="B247" t="s">
+        <v>70</v>
+      </c>
+      <c r="C247" t="s">
+        <v>13</v>
+      </c>
+      <c r="D247" t="s">
+        <v>9</v>
+      </c>
+      <c r="E247" t="s">
+        <v>9</v>
+      </c>
+      <c r="F247" t="s">
+        <v>9</v>
+      </c>
+      <c r="G247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>1021797</v>
+      </c>
+      <c r="B248" t="s">
+        <v>70</v>
+      </c>
+      <c r="C248" t="s">
+        <v>18</v>
+      </c>
+      <c r="D248" t="s">
+        <v>35</v>
+      </c>
+      <c r="E248" t="s">
+        <v>18</v>
+      </c>
+      <c r="F248" t="s">
+        <v>18</v>
+      </c>
+      <c r="G248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>1021790</v>
+      </c>
+      <c r="B249" t="s">
+        <v>70</v>
+      </c>
+      <c r="C249" t="s">
+        <v>28</v>
+      </c>
+      <c r="D249" t="s">
+        <v>20</v>
+      </c>
+      <c r="E249" t="s">
+        <v>20</v>
+      </c>
+      <c r="F249" t="s">
+        <v>20</v>
+      </c>
+      <c r="G249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>1021793</v>
+      </c>
+      <c r="B250" t="s">
+        <v>70</v>
+      </c>
+      <c r="C250" t="s">
+        <v>19</v>
+      </c>
+      <c r="D250" t="s">
+        <v>21</v>
+      </c>
+      <c r="E250" t="s">
+        <v>21</v>
+      </c>
+      <c r="F250" t="s">
+        <v>19</v>
+      </c>
+      <c r="G250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>1021796</v>
+      </c>
+      <c r="B251" t="s">
+        <v>70</v>
+      </c>
+      <c r="C251" t="s">
+        <v>12</v>
+      </c>
+      <c r="D251" t="s">
+        <v>32</v>
+      </c>
+      <c r="E251" t="s">
+        <v>32</v>
+      </c>
+      <c r="F251" t="s">
+        <v>32</v>
+      </c>
+      <c r="G251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>1021798</v>
+      </c>
+      <c r="B252" t="s">
+        <v>70</v>
+      </c>
+      <c r="C252" t="s">
+        <v>29</v>
+      </c>
+      <c r="D252" t="s">
+        <v>22</v>
+      </c>
+      <c r="E252" t="s">
+        <v>29</v>
+      </c>
+      <c r="F252" t="s">
+        <v>22</v>
+      </c>
+      <c r="G252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>1021799</v>
+      </c>
+      <c r="B253" t="s">
+        <v>71</v>
+      </c>
+      <c r="C253" t="s">
+        <v>9</v>
+      </c>
+      <c r="D253" t="s">
+        <v>11</v>
+      </c>
+      <c r="E253" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trying to implement ensemble learning with majority voting
</commit_message>
<xml_diff>
--- a/prediction_record.xlsx
+++ b/prediction_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0bd5acfa1e98a521/Documents/A-Z Machine Learning-Calebs-/A-Z_Machine-Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_174C5AA8D067C46F6D72103554322E3B7D88B6A9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3046F59-A911-4395-9E75-E8058ED28DA6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_58AD26DD502D95E5862D0B02027307055D082F26" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="2700" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="76">
   <si>
     <t>GameID</t>
   </si>
@@ -249,6 +249,18 @@
   </si>
   <si>
     <t>Tue, Feb 18, 2025</t>
+  </si>
+  <si>
+    <t>Wed, Feb 19, 2025</t>
+  </si>
+  <si>
+    <t>Fri, Feb 21, 2025</t>
+  </si>
+  <si>
+    <t>Sat, Feb 22, 2025</t>
+  </si>
+  <si>
+    <t>Sun, Feb 23, 2025</t>
   </si>
 </sst>
 </file>
@@ -634,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I253"/>
+  <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="I256" sqref="I256"/>
+    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="I271" sqref="I271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +716,7 @@
       </c>
       <c r="I2" s="2" t="str">
         <f>TEXT((SUM(G:G)/(COUNTA(G:G)-1)), "0.00%")</f>
-        <v>62.95%</v>
+        <v>62.41%</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -6471,7 +6483,570 @@
         <v>11</v>
       </c>
       <c r="E253" t="s">
+        <v>9</v>
+      </c>
+      <c r="F253" t="s">
+        <v>9</v>
+      </c>
+      <c r="G253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>1021800</v>
+      </c>
+      <c r="B254" t="s">
+        <v>72</v>
+      </c>
+      <c r="C254" t="s">
+        <v>27</v>
+      </c>
+      <c r="D254" t="s">
+        <v>13</v>
+      </c>
+      <c r="E254" t="s">
+        <v>27</v>
+      </c>
+      <c r="F254" t="s">
+        <v>13</v>
+      </c>
+      <c r="G254">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>1021801</v>
+      </c>
+      <c r="B255" t="s">
+        <v>72</v>
+      </c>
+      <c r="C255" t="s">
+        <v>10</v>
+      </c>
+      <c r="D255" t="s">
+        <v>32</v>
+      </c>
+      <c r="E255" t="s">
+        <v>32</v>
+      </c>
+      <c r="F255" t="s">
+        <v>32</v>
+      </c>
+      <c r="G255">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>1021802</v>
+      </c>
+      <c r="B256" t="s">
+        <v>73</v>
+      </c>
+      <c r="C256" t="s">
+        <v>9</v>
+      </c>
+      <c r="D256" t="s">
+        <v>32</v>
+      </c>
+      <c r="E256" t="s">
+        <v>9</v>
+      </c>
+      <c r="F256" t="s">
+        <v>32</v>
+      </c>
+      <c r="G256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>1021807</v>
+      </c>
+      <c r="B257" t="s">
+        <v>73</v>
+      </c>
+      <c r="C257" t="s">
         <v>11</v>
+      </c>
+      <c r="D257" t="s">
+        <v>14</v>
+      </c>
+      <c r="E257" t="s">
+        <v>11</v>
+      </c>
+      <c r="F257" t="s">
+        <v>11</v>
+      </c>
+      <c r="G257">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>1021810</v>
+      </c>
+      <c r="B258" t="s">
+        <v>73</v>
+      </c>
+      <c r="C258" t="s">
+        <v>12</v>
+      </c>
+      <c r="D258" t="s">
+        <v>10</v>
+      </c>
+      <c r="E258" t="s">
+        <v>12</v>
+      </c>
+      <c r="F258" t="s">
+        <v>10</v>
+      </c>
+      <c r="G258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>1021805</v>
+      </c>
+      <c r="B259" t="s">
+        <v>73</v>
+      </c>
+      <c r="C259" t="s">
+        <v>27</v>
+      </c>
+      <c r="D259" t="s">
+        <v>17</v>
+      </c>
+      <c r="E259" t="s">
+        <v>27</v>
+      </c>
+      <c r="F259" t="s">
+        <v>27</v>
+      </c>
+      <c r="G259">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>1021806</v>
+      </c>
+      <c r="B260" t="s">
+        <v>73</v>
+      </c>
+      <c r="C260" t="s">
+        <v>26</v>
+      </c>
+      <c r="D260" t="s">
+        <v>16</v>
+      </c>
+      <c r="E260" t="s">
+        <v>16</v>
+      </c>
+      <c r="F260" t="s">
+        <v>16</v>
+      </c>
+      <c r="G260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>1021808</v>
+      </c>
+      <c r="B261" t="s">
+        <v>73</v>
+      </c>
+      <c r="C261" t="s">
+        <v>15</v>
+      </c>
+      <c r="D261" t="s">
+        <v>13</v>
+      </c>
+      <c r="E261" t="s">
+        <v>13</v>
+      </c>
+      <c r="F261" t="s">
+        <v>13</v>
+      </c>
+      <c r="G261">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>1021812</v>
+      </c>
+      <c r="B262" t="s">
+        <v>73</v>
+      </c>
+      <c r="C262" t="s">
+        <v>24</v>
+      </c>
+      <c r="D262" t="s">
+        <v>21</v>
+      </c>
+      <c r="E262" t="s">
+        <v>21</v>
+      </c>
+      <c r="F262" t="s">
+        <v>24</v>
+      </c>
+      <c r="G262">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>1021803</v>
+      </c>
+      <c r="B263" t="s">
+        <v>73</v>
+      </c>
+      <c r="C263" t="s">
+        <v>22</v>
+      </c>
+      <c r="D263" t="s">
+        <v>19</v>
+      </c>
+      <c r="E263" t="s">
+        <v>19</v>
+      </c>
+      <c r="F263" t="s">
+        <v>22</v>
+      </c>
+      <c r="G263">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>1021804</v>
+      </c>
+      <c r="B264" t="s">
+        <v>73</v>
+      </c>
+      <c r="C264" t="s">
+        <v>28</v>
+      </c>
+      <c r="D264" t="s">
+        <v>18</v>
+      </c>
+      <c r="E264" t="s">
+        <v>18</v>
+      </c>
+      <c r="F264" t="s">
+        <v>18</v>
+      </c>
+      <c r="G264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>1021809</v>
+      </c>
+      <c r="B265" t="s">
+        <v>73</v>
+      </c>
+      <c r="C265" t="s">
+        <v>23</v>
+      </c>
+      <c r="D265" t="s">
+        <v>20</v>
+      </c>
+      <c r="E265" t="s">
+        <v>20</v>
+      </c>
+      <c r="F265" t="s">
+        <v>23</v>
+      </c>
+      <c r="G265">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>1021811</v>
+      </c>
+      <c r="B266" t="s">
+        <v>73</v>
+      </c>
+      <c r="C266" t="s">
+        <v>29</v>
+      </c>
+      <c r="D266" t="s">
+        <v>35</v>
+      </c>
+      <c r="E266" t="s">
+        <v>29</v>
+      </c>
+      <c r="F266" t="s">
+        <v>29</v>
+      </c>
+      <c r="G266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>1021816</v>
+      </c>
+      <c r="B267" t="s">
+        <v>74</v>
+      </c>
+      <c r="C267" t="s">
+        <v>10</v>
+      </c>
+      <c r="D267" t="s">
+        <v>11</v>
+      </c>
+      <c r="E267" t="s">
+        <v>11</v>
+      </c>
+      <c r="F267" t="s">
+        <v>11</v>
+      </c>
+      <c r="G267">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>1021814</v>
+      </c>
+      <c r="B268" t="s">
+        <v>74</v>
+      </c>
+      <c r="C268" t="s">
+        <v>14</v>
+      </c>
+      <c r="D268" t="s">
+        <v>32</v>
+      </c>
+      <c r="E268" t="s">
+        <v>32</v>
+      </c>
+      <c r="F268" t="s">
+        <v>32</v>
+      </c>
+      <c r="G268">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>1021818</v>
+      </c>
+      <c r="B269" t="s">
+        <v>74</v>
+      </c>
+      <c r="C269" t="s">
+        <v>12</v>
+      </c>
+      <c r="D269" t="s">
+        <v>9</v>
+      </c>
+      <c r="E269" t="s">
+        <v>9</v>
+      </c>
+      <c r="F269" t="s">
+        <v>12</v>
+      </c>
+      <c r="G269">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>1021813</v>
+      </c>
+      <c r="B270" t="s">
+        <v>74</v>
+      </c>
+      <c r="C270" t="s">
+        <v>26</v>
+      </c>
+      <c r="D270" t="s">
+        <v>17</v>
+      </c>
+      <c r="E270" t="s">
+        <v>26</v>
+      </c>
+      <c r="F270" t="s">
+        <v>26</v>
+      </c>
+      <c r="G270">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>1021815</v>
+      </c>
+      <c r="B271" t="s">
+        <v>74</v>
+      </c>
+      <c r="C271" t="s">
+        <v>19</v>
+      </c>
+      <c r="D271" t="s">
+        <v>24</v>
+      </c>
+      <c r="E271" t="s">
+        <v>19</v>
+      </c>
+      <c r="F271" t="s">
+        <v>19</v>
+      </c>
+      <c r="G271">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>1021817</v>
+      </c>
+      <c r="B272" t="s">
+        <v>74</v>
+      </c>
+      <c r="C272" t="s">
+        <v>21</v>
+      </c>
+      <c r="D272" t="s">
+        <v>22</v>
+      </c>
+      <c r="E272" t="s">
+        <v>22</v>
+      </c>
+      <c r="F272" t="s">
+        <v>21</v>
+      </c>
+      <c r="G272">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>1021819</v>
+      </c>
+      <c r="B273" t="s">
+        <v>74</v>
+      </c>
+      <c r="C273" t="s">
+        <v>20</v>
+      </c>
+      <c r="D273" t="s">
+        <v>23</v>
+      </c>
+      <c r="E273" t="s">
+        <v>23</v>
+      </c>
+      <c r="F273" t="s">
+        <v>20</v>
+      </c>
+      <c r="G273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>1021821</v>
+      </c>
+      <c r="B274" t="s">
+        <v>74</v>
+      </c>
+      <c r="C274" t="s">
+        <v>29</v>
+      </c>
+      <c r="D274" t="s">
+        <v>35</v>
+      </c>
+      <c r="E274" t="s">
+        <v>29</v>
+      </c>
+      <c r="F274" t="s">
+        <v>29</v>
+      </c>
+      <c r="G274">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>1021820</v>
+      </c>
+      <c r="B275" t="s">
+        <v>74</v>
+      </c>
+      <c r="C275" t="s">
+        <v>18</v>
+      </c>
+      <c r="D275" t="s">
+        <v>28</v>
+      </c>
+      <c r="E275" t="s">
+        <v>18</v>
+      </c>
+      <c r="F275" t="s">
+        <v>28</v>
+      </c>
+      <c r="G275">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>1021823</v>
+      </c>
+      <c r="B276" t="s">
+        <v>75</v>
+      </c>
+      <c r="C276" t="s">
+        <v>19</v>
+      </c>
+      <c r="D276" t="s">
+        <v>23</v>
+      </c>
+      <c r="E276" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>1021824</v>
+      </c>
+      <c r="B277" t="s">
+        <v>75</v>
+      </c>
+      <c r="C277" t="s">
+        <v>24</v>
+      </c>
+      <c r="D277" t="s">
+        <v>18</v>
+      </c>
+      <c r="E277" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>1021822</v>
+      </c>
+      <c r="B278" t="s">
+        <v>75</v>
+      </c>
+      <c r="C278" t="s">
+        <v>16</v>
+      </c>
+      <c r="D278" t="s">
+        <v>26</v>
+      </c>
+      <c r="E278" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed noneType error with powerplay goals
</commit_message>
<xml_diff>
--- a/prediction_record.xlsx
+++ b/prediction_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0bd5acfa1e98a521/Documents/A-Z Machine Learning-Calebs-/A-Z_Machine-Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_67058D0ED50A3BE5862D0B3582B02B1F5D0B60CA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C2B09F0-4EEB-4704-834D-821BBB64611F}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_44099BDFD30BCBE5862D0BF2EA372D555C0B1699" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{559433DA-76CF-4481-BD75-657BF5B45F47}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5415" yWindow="5415" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1873" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1944" uniqueCount="94">
   <si>
     <t>GameID</t>
   </si>
@@ -306,6 +306,15 @@
   </si>
   <si>
     <t>Sun, Mar 16, 2025</t>
+  </si>
+  <si>
+    <t>Tue, Mar 18, 2025</t>
+  </si>
+  <si>
+    <t>Fri, Mar 21, 2025</t>
+  </si>
+  <si>
+    <t>Wed, Mar 19, 2025</t>
   </si>
 </sst>
 </file>
@@ -691,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I375"/>
+  <dimension ref="A1:I390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A352" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G373" sqref="G373"/>
+    <sheetView tabSelected="1" topLeftCell="A364" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H383" sqref="H383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,7 +770,7 @@
       </c>
       <c r="I2" s="2" t="str">
         <f>TEXT((SUM(G:G)/(COUNTA(G:G)-1)), "0.00%")</f>
-        <v>62.87%</v>
+        <v>63.16%</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -9244,6 +9253,12 @@
       <c r="E371" t="s">
         <v>32</v>
       </c>
+      <c r="F371" t="s">
+        <v>16</v>
+      </c>
+      <c r="G371">
+        <v>0</v>
+      </c>
     </row>
     <row r="372" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A372">
@@ -9261,6 +9276,12 @@
       <c r="E372" t="s">
         <v>13</v>
       </c>
+      <c r="F372" t="s">
+        <v>13</v>
+      </c>
+      <c r="G372">
+        <v>1</v>
+      </c>
     </row>
     <row r="373" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A373">
@@ -9276,7 +9297,13 @@
         <v>18</v>
       </c>
       <c r="E373" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="F373" t="s">
+        <v>19</v>
+      </c>
+      <c r="G373">
+        <v>1</v>
       </c>
     </row>
     <row r="374" spans="1:7" x14ac:dyDescent="0.25">
@@ -9295,6 +9322,12 @@
       <c r="E374" t="s">
         <v>21</v>
       </c>
+      <c r="F374" t="s">
+        <v>21</v>
+      </c>
+      <c r="G374">
+        <v>1</v>
+      </c>
     </row>
     <row r="375" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A375">
@@ -9310,6 +9343,303 @@
         <v>22</v>
       </c>
       <c r="E375" t="s">
+        <v>23</v>
+      </c>
+      <c r="F375" t="s">
+        <v>22</v>
+      </c>
+      <c r="G375">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="376" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A376">
+        <v>1021923</v>
+      </c>
+      <c r="B376" t="s">
+        <v>91</v>
+      </c>
+      <c r="C376" t="s">
+        <v>11</v>
+      </c>
+      <c r="D376" t="s">
+        <v>14</v>
+      </c>
+      <c r="E376" t="s">
+        <v>11</v>
+      </c>
+      <c r="F376" t="s">
+        <v>11</v>
+      </c>
+      <c r="G376">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="377" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A377">
+        <v>1021924</v>
+      </c>
+      <c r="B377" t="s">
+        <v>91</v>
+      </c>
+      <c r="C377" t="s">
+        <v>10</v>
+      </c>
+      <c r="D377" t="s">
+        <v>12</v>
+      </c>
+      <c r="E377" t="s">
+        <v>12</v>
+      </c>
+      <c r="F377" t="s">
+        <v>10</v>
+      </c>
+      <c r="G377">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="378" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A378">
+        <v>1021922</v>
+      </c>
+      <c r="B378" t="s">
+        <v>91</v>
+      </c>
+      <c r="C378" t="s">
+        <v>17</v>
+      </c>
+      <c r="D378" t="s">
+        <v>29</v>
+      </c>
+      <c r="E378" t="s">
+        <v>29</v>
+      </c>
+      <c r="F378" t="s">
+        <v>29</v>
+      </c>
+      <c r="G378">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="379" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A379">
+        <v>1021925</v>
+      </c>
+      <c r="B379" t="s">
+        <v>93</v>
+      </c>
+      <c r="C379" t="s">
+        <v>9</v>
+      </c>
+      <c r="D379" t="s">
+        <v>13</v>
+      </c>
+      <c r="E379" t="s">
+        <v>13</v>
+      </c>
+      <c r="F379" t="s">
+        <v>13</v>
+      </c>
+      <c r="G379">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="380" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A380">
+        <v>1021926</v>
+      </c>
+      <c r="B380" t="s">
+        <v>93</v>
+      </c>
+      <c r="C380" t="s">
+        <v>32</v>
+      </c>
+      <c r="D380" t="s">
+        <v>15</v>
+      </c>
+      <c r="E380" t="s">
+        <v>32</v>
+      </c>
+      <c r="F380" t="s">
+        <v>32</v>
+      </c>
+      <c r="G380">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="381" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A381">
+        <v>1021927</v>
+      </c>
+      <c r="B381" t="s">
+        <v>93</v>
+      </c>
+      <c r="C381" t="s">
+        <v>28</v>
+      </c>
+      <c r="D381" t="s">
+        <v>29</v>
+      </c>
+      <c r="E381" t="s">
+        <v>29</v>
+      </c>
+      <c r="F381" t="s">
+        <v>29</v>
+      </c>
+      <c r="G381">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="382" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A382">
+        <v>1021928</v>
+      </c>
+      <c r="B382" t="s">
+        <v>92</v>
+      </c>
+      <c r="C382" t="s">
+        <v>9</v>
+      </c>
+      <c r="D382" t="s">
+        <v>10</v>
+      </c>
+      <c r="E382" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A383">
+        <v>1021931</v>
+      </c>
+      <c r="B383" t="s">
+        <v>92</v>
+      </c>
+      <c r="C383" t="s">
+        <v>27</v>
+      </c>
+      <c r="D383" t="s">
+        <v>16</v>
+      </c>
+      <c r="E383" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A384">
+        <v>1021932</v>
+      </c>
+      <c r="B384" t="s">
+        <v>92</v>
+      </c>
+      <c r="C384" t="s">
+        <v>12</v>
+      </c>
+      <c r="D384" t="s">
+        <v>14</v>
+      </c>
+      <c r="E384" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="385" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A385">
+        <v>1021935</v>
+      </c>
+      <c r="B385" t="s">
+        <v>92</v>
+      </c>
+      <c r="C385" t="s">
+        <v>13</v>
+      </c>
+      <c r="D385" t="s">
+        <v>11</v>
+      </c>
+      <c r="E385" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="386" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A386">
+        <v>1021930</v>
+      </c>
+      <c r="B386" t="s">
+        <v>92</v>
+      </c>
+      <c r="C386" t="s">
+        <v>17</v>
+      </c>
+      <c r="D386" t="s">
+        <v>18</v>
+      </c>
+      <c r="E386" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A387">
+        <v>1021933</v>
+      </c>
+      <c r="B387" t="s">
+        <v>92</v>
+      </c>
+      <c r="C387" t="s">
+        <v>19</v>
+      </c>
+      <c r="D387" t="s">
+        <v>20</v>
+      </c>
+      <c r="E387" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="388" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A388">
+        <v>1021934</v>
+      </c>
+      <c r="B388" t="s">
+        <v>92</v>
+      </c>
+      <c r="C388" t="s">
+        <v>35</v>
+      </c>
+      <c r="D388" t="s">
+        <v>29</v>
+      </c>
+      <c r="E388" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="389" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A389">
+        <v>1021929</v>
+      </c>
+      <c r="B389" t="s">
+        <v>92</v>
+      </c>
+      <c r="C389" t="s">
+        <v>22</v>
+      </c>
+      <c r="D389" t="s">
+        <v>24</v>
+      </c>
+      <c r="E389" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A390">
+        <v>1021936</v>
+      </c>
+      <c r="B390" t="s">
+        <v>92</v>
+      </c>
+      <c r="C390" t="s">
+        <v>23</v>
+      </c>
+      <c r="D390" t="s">
+        <v>21</v>
+      </c>
+      <c r="E390" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update predictions for playoffs
</commit_message>
<xml_diff>
--- a/prediction_record.xlsx
+++ b/prediction_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0bd5acfa1e98a521/Documents/A-Z Machine Learning-Calebs-/A-Z_Machine-Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_44099BDFD30BCBE5862D0BF2EA372D555C0B1699" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{559433DA-76CF-4481-BD75-657BF5B45F47}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_140FBDF4167F5C6F6D72103554322E3BFD04212C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C897BE36-339D-4062-8BD2-79317B9FAF59}"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="5415" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6300" yWindow="1530" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1944" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2055" uniqueCount="97">
   <si>
     <t>GameID</t>
   </si>
@@ -311,10 +311,19 @@
     <t>Tue, Mar 18, 2025</t>
   </si>
   <si>
+    <t>Wed, Mar 19, 2025</t>
+  </si>
+  <si>
     <t>Fri, Mar 21, 2025</t>
   </si>
   <si>
-    <t>Wed, Mar 19, 2025</t>
+    <t>Sat, Mar 22, 2025</t>
+  </si>
+  <si>
+    <t>Fri, Mar 28, 2025</t>
+  </si>
+  <si>
+    <t>Sun, Mar 23, 2025</t>
   </si>
 </sst>
 </file>
@@ -381,6 +390,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -700,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I390"/>
+  <dimension ref="A1:I412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A364" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H383" sqref="H383"/>
+    <sheetView tabSelected="1" topLeftCell="A388" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D418" sqref="D418"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +783,7 @@
       </c>
       <c r="I2" s="2" t="str">
         <f>TEXT((SUM(G:G)/(COUNTA(G:G)-1)), "0.00%")</f>
-        <v>63.16%</v>
+        <v>63.28%</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -9426,7 +9439,7 @@
         <v>1021925</v>
       </c>
       <c r="B379" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C379" t="s">
         <v>9</v>
@@ -9449,7 +9462,7 @@
         <v>1021926</v>
       </c>
       <c r="B380" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C380" t="s">
         <v>32</v>
@@ -9472,7 +9485,7 @@
         <v>1021927</v>
       </c>
       <c r="B381" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C381" t="s">
         <v>28</v>
@@ -9495,7 +9508,7 @@
         <v>1021928</v>
       </c>
       <c r="B382" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C382" t="s">
         <v>9</v>
@@ -9504,7 +9517,13 @@
         <v>10</v>
       </c>
       <c r="E382" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="F382" t="s">
+        <v>9</v>
+      </c>
+      <c r="G382">
+        <v>1</v>
       </c>
     </row>
     <row r="383" spans="1:7" x14ac:dyDescent="0.25">
@@ -9512,7 +9531,7 @@
         <v>1021931</v>
       </c>
       <c r="B383" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C383" t="s">
         <v>27</v>
@@ -9521,7 +9540,13 @@
         <v>16</v>
       </c>
       <c r="E383" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="F383" t="s">
+        <v>27</v>
+      </c>
+      <c r="G383">
+        <v>1</v>
       </c>
     </row>
     <row r="384" spans="1:7" x14ac:dyDescent="0.25">
@@ -9529,7 +9554,7 @@
         <v>1021932</v>
       </c>
       <c r="B384" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C384" t="s">
         <v>12</v>
@@ -9538,15 +9563,21 @@
         <v>14</v>
       </c>
       <c r="E384" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="385" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="F384" t="s">
+        <v>12</v>
+      </c>
+      <c r="G384">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="385" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>1021935</v>
       </c>
       <c r="B385" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C385" t="s">
         <v>13</v>
@@ -9557,13 +9588,19 @@
       <c r="E385" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F385" t="s">
+        <v>11</v>
+      </c>
+      <c r="G385">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>1021930</v>
       </c>
       <c r="B386" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C386" t="s">
         <v>17</v>
@@ -9574,13 +9611,19 @@
       <c r="E386" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F386" t="s">
+        <v>18</v>
+      </c>
+      <c r="G386">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>1021933</v>
       </c>
       <c r="B387" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C387" t="s">
         <v>19</v>
@@ -9591,13 +9634,19 @@
       <c r="E387" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F387" t="s">
+        <v>20</v>
+      </c>
+      <c r="G387">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>1021934</v>
       </c>
       <c r="B388" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C388" t="s">
         <v>35</v>
@@ -9608,13 +9657,19 @@
       <c r="E388" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F388" t="s">
+        <v>29</v>
+      </c>
+      <c r="G388">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="389" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>1021929</v>
       </c>
       <c r="B389" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C389" t="s">
         <v>22</v>
@@ -9625,13 +9680,19 @@
       <c r="E389" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F389" t="s">
+        <v>22</v>
+      </c>
+      <c r="G389">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="390" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>1021936</v>
       </c>
       <c r="B390" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C390" t="s">
         <v>23</v>
@@ -9641,6 +9702,470 @@
       </c>
       <c r="E390" t="s">
         <v>23</v>
+      </c>
+      <c r="F390" t="s">
+        <v>21</v>
+      </c>
+      <c r="G390">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="391" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A391">
+        <v>1021942</v>
+      </c>
+      <c r="B391" t="s">
+        <v>94</v>
+      </c>
+      <c r="C391" t="s">
+        <v>10</v>
+      </c>
+      <c r="D391" t="s">
+        <v>9</v>
+      </c>
+      <c r="E391" t="s">
+        <v>9</v>
+      </c>
+      <c r="F391" t="s">
+        <v>9</v>
+      </c>
+      <c r="G391">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="392" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A392">
+        <v>1021938</v>
+      </c>
+      <c r="B392" t="s">
+        <v>94</v>
+      </c>
+      <c r="C392" t="s">
+        <v>26</v>
+      </c>
+      <c r="D392" t="s">
+        <v>27</v>
+      </c>
+      <c r="E392" t="s">
+        <v>26</v>
+      </c>
+      <c r="F392" t="s">
+        <v>26</v>
+      </c>
+      <c r="G392">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="393" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A393">
+        <v>1021939</v>
+      </c>
+      <c r="B393" t="s">
+        <v>94</v>
+      </c>
+      <c r="C393" t="s">
+        <v>11</v>
+      </c>
+      <c r="D393" t="s">
+        <v>13</v>
+      </c>
+      <c r="E393" t="s">
+        <v>13</v>
+      </c>
+      <c r="F393" t="s">
+        <v>11</v>
+      </c>
+      <c r="G393">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="394" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A394">
+        <v>1021940</v>
+      </c>
+      <c r="B394" t="s">
+        <v>94</v>
+      </c>
+      <c r="C394" t="s">
+        <v>35</v>
+      </c>
+      <c r="D394" t="s">
+        <v>29</v>
+      </c>
+      <c r="E394" t="s">
+        <v>29</v>
+      </c>
+      <c r="F394" t="s">
+        <v>35</v>
+      </c>
+      <c r="G394">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="395" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A395">
+        <v>1021941</v>
+      </c>
+      <c r="B395" t="s">
+        <v>94</v>
+      </c>
+      <c r="C395" t="s">
+        <v>15</v>
+      </c>
+      <c r="D395" t="s">
+        <v>32</v>
+      </c>
+      <c r="E395" t="s">
+        <v>32</v>
+      </c>
+      <c r="F395" t="s">
+        <v>32</v>
+      </c>
+      <c r="G395">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="396" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A396">
+        <v>1021944</v>
+      </c>
+      <c r="B396" t="s">
+        <v>94</v>
+      </c>
+      <c r="C396" t="s">
+        <v>14</v>
+      </c>
+      <c r="D396" t="s">
+        <v>12</v>
+      </c>
+      <c r="E396" t="s">
+        <v>12</v>
+      </c>
+      <c r="F396" t="s">
+        <v>14</v>
+      </c>
+      <c r="G396">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="397" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A397">
+        <v>1021946</v>
+      </c>
+      <c r="B397" t="s">
+        <v>94</v>
+      </c>
+      <c r="C397" t="s">
+        <v>24</v>
+      </c>
+      <c r="D397" t="s">
+        <v>22</v>
+      </c>
+      <c r="E397" t="s">
+        <v>22</v>
+      </c>
+      <c r="F397" t="s">
+        <v>22</v>
+      </c>
+      <c r="G397">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="398" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A398">
+        <v>1021937</v>
+      </c>
+      <c r="B398" t="s">
+        <v>94</v>
+      </c>
+      <c r="C398" t="s">
+        <v>28</v>
+      </c>
+      <c r="D398" t="s">
+        <v>17</v>
+      </c>
+      <c r="E398" t="s">
+        <v>17</v>
+      </c>
+      <c r="F398" t="s">
+        <v>28</v>
+      </c>
+      <c r="G398">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="399" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A399">
+        <v>1021943</v>
+      </c>
+      <c r="B399" t="s">
+        <v>94</v>
+      </c>
+      <c r="C399" t="s">
+        <v>21</v>
+      </c>
+      <c r="D399" t="s">
+        <v>19</v>
+      </c>
+      <c r="E399" t="s">
+        <v>21</v>
+      </c>
+      <c r="F399" t="s">
+        <v>21</v>
+      </c>
+      <c r="G399">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="400" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A400">
+        <v>1021945</v>
+      </c>
+      <c r="B400" t="s">
+        <v>94</v>
+      </c>
+      <c r="C400" t="s">
+        <v>20</v>
+      </c>
+      <c r="D400" t="s">
+        <v>23</v>
+      </c>
+      <c r="E400" t="s">
+        <v>23</v>
+      </c>
+      <c r="F400" t="s">
+        <v>23</v>
+      </c>
+      <c r="G400">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="401" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A401">
+        <v>1021948</v>
+      </c>
+      <c r="B401" t="s">
+        <v>96</v>
+      </c>
+      <c r="C401" t="s">
+        <v>16</v>
+      </c>
+      <c r="D401" t="s">
+        <v>15</v>
+      </c>
+      <c r="E401" t="s">
+        <v>16</v>
+      </c>
+      <c r="F401" t="s">
+        <v>16</v>
+      </c>
+      <c r="G401">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="402" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A402">
+        <v>1021947</v>
+      </c>
+      <c r="B402" t="s">
+        <v>96</v>
+      </c>
+      <c r="C402" t="s">
+        <v>32</v>
+      </c>
+      <c r="D402" t="s">
+        <v>26</v>
+      </c>
+      <c r="E402" t="s">
+        <v>26</v>
+      </c>
+      <c r="F402" t="s">
+        <v>26</v>
+      </c>
+      <c r="G402">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A403">
+        <v>1021949</v>
+      </c>
+      <c r="B403" t="s">
+        <v>96</v>
+      </c>
+      <c r="C403" t="s">
+        <v>18</v>
+      </c>
+      <c r="D403" t="s">
+        <v>28</v>
+      </c>
+      <c r="E403" t="s">
+        <v>18</v>
+      </c>
+      <c r="F403" t="s">
+        <v>18</v>
+      </c>
+      <c r="G403">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="404" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A404">
+        <v>1021891</v>
+      </c>
+      <c r="B404" t="s">
+        <v>96</v>
+      </c>
+      <c r="C404" t="s">
+        <v>20</v>
+      </c>
+      <c r="D404" t="s">
+        <v>21</v>
+      </c>
+      <c r="E404" t="s">
+        <v>21</v>
+      </c>
+      <c r="F404" t="s">
+        <v>21</v>
+      </c>
+      <c r="G404">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="405" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A405">
+        <v>1021963</v>
+      </c>
+      <c r="B405" t="s">
+        <v>95</v>
+      </c>
+      <c r="C405" t="s">
+        <v>32</v>
+      </c>
+      <c r="D405" t="s">
+        <v>13</v>
+      </c>
+      <c r="E405" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="406" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A406">
+        <v>1021965</v>
+      </c>
+      <c r="B406" t="s">
+        <v>95</v>
+      </c>
+      <c r="C406" t="s">
+        <v>27</v>
+      </c>
+      <c r="D406" t="s">
+        <v>9</v>
+      </c>
+      <c r="E406" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="407" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A407">
+        <v>1021990</v>
+      </c>
+      <c r="B407" t="s">
+        <v>95</v>
+      </c>
+      <c r="C407" t="s">
+        <v>11</v>
+      </c>
+      <c r="D407" t="s">
+        <v>16</v>
+      </c>
+      <c r="E407" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="408" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A408">
+        <v>1022005</v>
+      </c>
+      <c r="B408" t="s">
+        <v>95</v>
+      </c>
+      <c r="C408" t="s">
+        <v>26</v>
+      </c>
+      <c r="D408" t="s">
+        <v>12</v>
+      </c>
+      <c r="E408" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="409" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A409">
+        <v>1021976</v>
+      </c>
+      <c r="B409" t="s">
+        <v>95</v>
+      </c>
+      <c r="C409" t="s">
+        <v>35</v>
+      </c>
+      <c r="D409" t="s">
+        <v>19</v>
+      </c>
+      <c r="E409" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="410" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A410">
+        <v>1021997</v>
+      </c>
+      <c r="B410" t="s">
+        <v>95</v>
+      </c>
+      <c r="C410" t="s">
+        <v>18</v>
+      </c>
+      <c r="D410" t="s">
+        <v>23</v>
+      </c>
+      <c r="E410" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="411" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A411">
+        <v>1021961</v>
+      </c>
+      <c r="B411" t="s">
+        <v>95</v>
+      </c>
+      <c r="C411" t="s">
+        <v>22</v>
+      </c>
+      <c r="D411" t="s">
+        <v>21</v>
+      </c>
+      <c r="E411" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="412" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A412">
+        <v>1021974</v>
+      </c>
+      <c r="B412" t="s">
+        <v>95</v>
+      </c>
+      <c r="C412" t="s">
+        <v>29</v>
+      </c>
+      <c r="D412" t="s">
+        <v>20</v>
+      </c>
+      <c r="E412" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update K and predictions
Going to try and use the last 15 games to make a prediction during playoffs, as opposed to 5
</commit_message>
<xml_diff>
--- a/prediction_record.xlsx
+++ b/prediction_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0bd5acfa1e98a521/Documents/A-Z Machine Learning-Calebs-/A-Z_Machine-Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_4AB56917522B4BE4862D0B8622F0060D5D0B64F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_39493F8A532CCBE5862D0BBC3AF139AF5D0B09C9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A70F5DF8-C9E4-40A9-9E48-76614CB6F853}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10785" yWindow="2235" windowWidth="17535" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2087" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2101" uniqueCount="99">
   <si>
     <t>GameID</t>
   </si>
@@ -327,6 +327,9 @@
   </si>
   <si>
     <t>Sat, Mar 29, 2025</t>
+  </si>
+  <si>
+    <t>Sun, Mar 30, 2025</t>
   </si>
 </sst>
 </file>
@@ -712,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I418"/>
+  <dimension ref="A1:I420"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A400" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F417" sqref="F417"/>
+    <sheetView tabSelected="1" topLeftCell="B394" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H413" sqref="H413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,7 +785,7 @@
       </c>
       <c r="I2" s="2" t="str">
         <f>TEXT((SUM(G:G)/(COUNTA(G:G)-1)), "0.00%")</f>
-        <v>63.02%</v>
+        <v>63.07%</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -10229,7 +10232,13 @@
         <v>9</v>
       </c>
       <c r="E413" t="s">
-        <v>9</v>
+        <v>27</v>
+      </c>
+      <c r="F413" t="s">
+        <v>27</v>
+      </c>
+      <c r="G413">
+        <v>1</v>
       </c>
     </row>
     <row r="414" spans="1:7" x14ac:dyDescent="0.25">
@@ -10248,6 +10257,12 @@
       <c r="E414" t="s">
         <v>19</v>
       </c>
+      <c r="F414" t="s">
+        <v>19</v>
+      </c>
+      <c r="G414">
+        <v>1</v>
+      </c>
     </row>
     <row r="415" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A415">
@@ -10265,6 +10280,12 @@
       <c r="E415" t="s">
         <v>16</v>
       </c>
+      <c r="F415" t="s">
+        <v>11</v>
+      </c>
+      <c r="G415">
+        <v>0</v>
+      </c>
     </row>
     <row r="416" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A416">
@@ -10282,8 +10303,14 @@
       <c r="E416" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F416" t="s">
+        <v>26</v>
+      </c>
+      <c r="G416">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="417" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A417">
         <v>1021962</v>
       </c>
@@ -10299,8 +10326,14 @@
       <c r="E417" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F417" t="s">
+        <v>22</v>
+      </c>
+      <c r="G417">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="418" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A418">
         <v>1021975</v>
       </c>
@@ -10315,6 +10348,46 @@
       </c>
       <c r="E418" t="s">
         <v>29</v>
+      </c>
+      <c r="F418" t="s">
+        <v>29</v>
+      </c>
+      <c r="G418">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="419" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A419">
+        <v>1021964</v>
+      </c>
+      <c r="B419" t="s">
+        <v>98</v>
+      </c>
+      <c r="C419" t="s">
+        <v>32</v>
+      </c>
+      <c r="D419" t="s">
+        <v>13</v>
+      </c>
+      <c r="E419" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="420" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A420">
+        <v>1021998</v>
+      </c>
+      <c r="B420" t="s">
+        <v>98</v>
+      </c>
+      <c r="C420" t="s">
+        <v>18</v>
+      </c>
+      <c r="D420" t="s">
+        <v>23</v>
+      </c>
+      <c r="E420" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made the train/test into a Flask microservice
This will be used later for a Hackathon. I will be building a tool off of this project, so its not cheating :)
</commit_message>
<xml_diff>
--- a/prediction_record.xlsx
+++ b/prediction_record.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -458,10 +458,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I479"/>
+  <dimension ref="A1:I481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A448" zoomScale="114" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I481" sqref="I481"/>
+      <selection activeCell="K475" sqref="K475"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -16256,8 +16256,13 @@
           <t>Medicine Hat Tigers</t>
         </is>
       </c>
-      <c r="F478" t="n">
-        <v/>
+      <c r="F478" t="inlineStr">
+        <is>
+          <t>Medicine Hat Tigers</t>
+        </is>
+      </c>
+      <c r="G478" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="479">
@@ -16284,7 +16289,73 @@
           <t>Spokane Chiefs</t>
         </is>
       </c>
-      <c r="F479" t="n">
+      <c r="F479" t="inlineStr">
+        <is>
+          <t>Spokane Chiefs</t>
+        </is>
+      </c>
+      <c r="G479" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="n">
+        <v>1022048</v>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Thu, May 1, 2025</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>Portland Winterhawks</t>
+        </is>
+      </c>
+      <c r="D480" t="inlineStr">
+        <is>
+          <t>Spokane Chiefs</t>
+        </is>
+      </c>
+      <c r="E480" t="inlineStr">
+        <is>
+          <t>Spokane Chiefs</t>
+        </is>
+      </c>
+      <c r="F480" t="inlineStr">
+        <is>
+          <t>Spokane Chiefs</t>
+        </is>
+      </c>
+      <c r="G480" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="n">
+        <v>1022060</v>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Fri, May 9, 2025</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>Medicine Hat Tigers</t>
+        </is>
+      </c>
+      <c r="D481" t="inlineStr">
+        <is>
+          <t>Spokane Chiefs</t>
+        </is>
+      </c>
+      <c r="E481" t="inlineStr">
+        <is>
+          <t>Spokane Chiefs</t>
+        </is>
+      </c>
+      <c r="F481" t="n">
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Now saved in user friendly csv file to view predictions quickly
</commit_message>
<xml_diff>
--- a/prediction_record.xlsx
+++ b/prediction_record.xlsx
@@ -458,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I485"/>
+  <dimension ref="A1:I486"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A463" zoomScale="114" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B486" sqref="B486"/>
@@ -16496,6 +16496,34 @@
         <v>1</v>
       </c>
     </row>
+    <row r="486">
+      <c r="A486" t="n">
+        <v>1022067</v>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Sun, Aug 31, 2025</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>Wenatchee Wild</t>
+        </is>
+      </c>
+      <c r="D486" t="inlineStr">
+        <is>
+          <t>Tri-City Americans</t>
+        </is>
+      </c>
+      <c r="E486" t="inlineStr">
+        <is>
+          <t>Wenatchee Wild</t>
+        </is>
+      </c>
+      <c r="F486" t="n">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed error with calculating avgs with a new team in the league
</commit_message>
<xml_diff>
--- a/prediction_record.xlsx
+++ b/prediction_record.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -458,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I489"/>
+  <dimension ref="A1:I494"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A463" zoomScale="114" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B486" sqref="B486"/>
@@ -16553,8 +16553,13 @@
           <t>Prince Albert Raiders</t>
         </is>
       </c>
-      <c r="F487" t="n">
-        <v/>
+      <c r="F487" t="inlineStr">
+        <is>
+          <t>Saskatoon Blades</t>
+        </is>
+      </c>
+      <c r="G487" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="488">
@@ -16581,8 +16586,13 @@
           <t>Medicine Hat Tigers</t>
         </is>
       </c>
-      <c r="F488" t="n">
-        <v/>
+      <c r="F488" t="inlineStr">
+        <is>
+          <t>Medicine Hat Tigers</t>
+        </is>
+      </c>
+      <c r="G488" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="489">
@@ -16609,7 +16619,152 @@
           <t>Everett Silvertips</t>
         </is>
       </c>
-      <c r="F489" t="n">
+      <c r="F489" t="inlineStr">
+        <is>
+          <t>Everett Silvertips</t>
+        </is>
+      </c>
+      <c r="G489" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="n">
+        <v>1022074</v>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Wed, Sep 3, 2025</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>Prince Albert Raiders</t>
+        </is>
+      </c>
+      <c r="D490" t="inlineStr">
+        <is>
+          <t>Saskatoon Blades</t>
+        </is>
+      </c>
+      <c r="E490" t="inlineStr">
+        <is>
+          <t>Saskatoon Blades</t>
+        </is>
+      </c>
+      <c r="F490" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="n">
+        <v>1022071</v>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Wed, Sep 3, 2025</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>Lethbridge Hurricanes</t>
+        </is>
+      </c>
+      <c r="D491" t="inlineStr">
+        <is>
+          <t>Calgary Hitmen</t>
+        </is>
+      </c>
+      <c r="E491" t="inlineStr">
+        <is>
+          <t>Calgary Hitmen</t>
+        </is>
+      </c>
+      <c r="F491" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="n">
+        <v>1022075</v>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Wed, Sep 3, 2025</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>Swift Current Broncos</t>
+        </is>
+      </c>
+      <c r="D492" t="inlineStr">
+        <is>
+          <t>Regina Pats</t>
+        </is>
+      </c>
+      <c r="E492" t="inlineStr">
+        <is>
+          <t>Swift Current Broncos</t>
+        </is>
+      </c>
+      <c r="F492" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="n">
+        <v>1022072</v>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Wed, Sep 3, 2025</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>Kamloops Blazers</t>
+        </is>
+      </c>
+      <c r="D493" t="inlineStr">
+        <is>
+          <t>Vancouver Giants</t>
+        </is>
+      </c>
+      <c r="E493" t="inlineStr">
+        <is>
+          <t>Vancouver Giants</t>
+        </is>
+      </c>
+      <c r="F493" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="n">
+        <v>1022073</v>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Wed, Sep 3, 2025</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>Kelowna Rockets</t>
+        </is>
+      </c>
+      <c r="D494" t="inlineStr">
+        <is>
+          <t>Penticton Vees</t>
+        </is>
+      </c>
+      <c r="E494" t="inlineStr">
+        <is>
+          <t>Penticton Vees</t>
+        </is>
+      </c>
+      <c r="F494" t="n">
         <v/>
       </c>
     </row>

</xml_diff>